<commit_message>
Remove moderate option from climate_zone
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerator_types/forms/refrigerator_types/refrigerator_types.xlsx
+++ b/app/config/tables/refrigerator_types/forms/refrigerator_types/refrigerator_types.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\cold-chain-app-designer\app\config\tables\refrigerator_types\forms\refrigerator_types\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26380" windowHeight="13940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26385" windowHeight="13935" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="properties" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="166">
   <si>
     <t>comments</t>
   </si>
@@ -370,12 +375,6 @@
   </si>
   <si>
     <t>Frigorífico termal</t>
-  </si>
-  <si>
-    <t>moderate</t>
-  </si>
-  <si>
-    <t>Moderate</t>
   </si>
   <si>
     <t>temperate</t>
@@ -534,7 +533,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -727,6 +726,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1054,27 +1061,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="22.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="22.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="43.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.125" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
+    <col min="8" max="8" width="20.125" customWidth="1"/>
+    <col min="9" max="9" width="43.375" customWidth="1"/>
     <col min="10" max="10" width="35" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="19.625" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>13</v>
@@ -1131,7 +1138,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1157,7 +1164,7 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1183,7 +1190,7 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>24</v>
@@ -1197,7 +1204,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1223,7 +1230,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1249,7 +1256,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
         <v>13</v>
@@ -1265,7 +1272,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="9" spans="1:13" s="9" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1294,7 +1301,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1320,7 +1327,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1346,7 +1353,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1384,7 +1391,7 @@
       <c r="J13" s="9"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:13" s="9" customFormat="1" ht="12">
+    <row r="14" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1410,14 +1417,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="9" customFormat="1" ht="12">
+    <row r="15" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:13" s="9" customFormat="1" ht="12">
+    <row r="16" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1443,7 +1450,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" ht="12">
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1469,7 +1476,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="9" customFormat="1" ht="12">
+    <row r="18" spans="1:10" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
         <v>24</v>
@@ -1496,21 +1503,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK18"/>
+  <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="10" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" style="10" customWidth="1"/>
-    <col min="4" max="1025" width="17.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="27.625" style="10" customWidth="1"/>
+    <col min="4" max="1025" width="17.125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.25" customHeight="1">
+    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>77</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19" customHeight="1">
+    <row r="2" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>59</v>
       </c>
@@ -1538,7 +1545,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.25" customHeight="1">
+    <row r="3" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>59</v>
       </c>
@@ -1552,7 +1559,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>59</v>
       </c>
@@ -1566,7 +1573,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19" customHeight="1">
+    <row r="5" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>59</v>
       </c>
@@ -1580,7 +1587,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22" customHeight="1">
+    <row r="6" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>59</v>
       </c>
@@ -1594,7 +1601,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1">
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>66</v>
       </c>
@@ -1608,7 +1615,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1">
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>66</v>
       </c>
@@ -1622,7 +1629,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1">
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>66</v>
       </c>
@@ -1636,7 +1643,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22" customHeight="1">
+    <row r="11" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>66</v>
       </c>
@@ -1650,7 +1657,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>66</v>
       </c>
@@ -1664,7 +1671,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20" customHeight="1">
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>66</v>
       </c>
@@ -1678,7 +1685,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20" customHeight="1">
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>66</v>
       </c>
@@ -1692,7 +1699,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>71</v>
       </c>
@@ -1703,35 +1710,21 @@
         <v>116</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="19" customHeight="1">
-      <c r="A18" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1749,166 +1742,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
         <v>123</v>
-      </c>
-      <c r="B1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" t="s">
-        <v>125</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>127</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>128</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>129</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
         <v>130</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4" t="s">
         <v>128</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="E6" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="E7" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="14" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="B8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="14" t="s">
+      <c r="D8" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="14" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1930,19 +1923,19 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1951,84 +1944,84 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>149</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>151</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>153</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>154</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30">
-      <c r="A6" s="16" t="s">
-        <v>157</v>
       </c>
       <c r="B6" s="6" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" s="17">
         <v>20170804</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" t="s">
         <v>160</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>161</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E10" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="F10" t="s">
         <v>163</v>
-      </c>
-      <c r="E10" t="s">
-        <v>164</v>
-      </c>
-      <c r="F10" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add refrigerator and freezer to the refrigerator types
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerator_types/forms/refrigerator_types/refrigerator_types.xlsx
+++ b/app/config/tables/refrigerator_types/forms/refrigerator_types/refrigerator_types.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26390" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26390" windowHeight="13940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
   <si>
     <t>comments</t>
   </si>
@@ -528,6 +528,33 @@
   </si>
   <si>
     <t>(litros)</t>
+  </si>
+  <si>
+    <t>refrigerator</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Frigorífico</t>
+  </si>
+  <si>
+    <t>freezer</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Congelador</t>
+  </si>
+  <si>
+    <t>refrigerator_freezer</t>
+  </si>
+  <si>
+    <t>Refrigerator/Freezer</t>
+  </si>
+  <si>
+    <t>Frigorífico/Congelador</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -1503,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1541,8 @@
     <col min="1" max="1" width="17.08203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="10" customWidth="1"/>
     <col min="3" max="3" width="27.58203125" style="10" customWidth="1"/>
-    <col min="4" max="1025" width="17.08203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.75" style="10" customWidth="1"/>
+    <col min="5" max="1025" width="17.08203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -1699,31 +1727,73 @@
         <v>112</v>
       </c>
     </row>
+    <row r="15" spans="1:4" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="16" spans="1:4" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+    <row r="20" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>